<commit_message>
3 Extra page added
</commit_message>
<xml_diff>
--- a/Financial Statement.xlsx
+++ b/Financial Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zoomcharts-my.sharepoint.com/personal/una_zoomcharts_com/Documents/Product_team/challenge/income_expense/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\_Portfolio Project Github\_Financial Dashboard\Financial_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="8_{047DCD00-26C3-476B-B396-74C3FDBD83AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D63164EC-D1B1-409B-ABF7-053FA808C71D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3701BFE5-6D3B-4383-89DD-2923ED596CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{03D87DC1-F306-4581-B651-66977685B5D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{03D87DC1-F306-4581-B651-66977685B5D8}"/>
   </bookViews>
   <sheets>
     <sheet name="revenue_expense" sheetId="1" r:id="rId1"/>
@@ -477,10 +477,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -493,10 +493,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -840,7 +836,7 @@
   <dimension ref="A1:I581"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>